<commit_message>
new update week 8
</commit_message>
<xml_diff>
--- a/report moi tuan/tuan 7/1159032-1359035-1359037-1359038.xlsx
+++ b/report moi tuan/tuan 7/1159032-1359035-1359037-1359038.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\son long\Documents\PM---Group-10\report moi tuan\tuan 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\son long\Documents\PM---Group-10\report moi tuan\tuan 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng quan" sheetId="4" r:id="rId1"/>
     <sheet name="Chi tiết" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="73">
   <si>
     <t>MSSV</t>
   </si>
@@ -177,10 +177,73 @@
     <t>Search Servlet</t>
   </si>
   <si>
-    <t>14/6/2016</t>
-  </si>
-  <si>
-    <t>Search jsp</t>
+    <t>Quản lý thông tin thành viên</t>
+  </si>
+  <si>
+    <t>Active account</t>
+  </si>
+  <si>
+    <t>Deactive account</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa thông tin tài khoản</t>
+  </si>
+  <si>
+    <t>Xoá tài khoản thành viên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiết kế giỏ hàng </t>
+  </si>
+  <si>
+    <t>Thêm sản phẩm vào giỏ hàng</t>
+  </si>
+  <si>
+    <t>Thanh toán giỏ hàng</t>
+  </si>
+  <si>
+    <t>Cộng nhiều sản phẩm</t>
+  </si>
+  <si>
+    <t>Đặt điều kiện cho giỏ hàng (không được dưới 0 sản phẩm)</t>
+  </si>
+  <si>
+    <t>15/6/2016</t>
+  </si>
+  <si>
+    <t>17/6/2016</t>
+  </si>
+  <si>
+    <t>19/6/2016</t>
+  </si>
+  <si>
+    <t>21/6/2016</t>
+  </si>
+  <si>
+    <t>23/6/2016</t>
+  </si>
+  <si>
+    <t>24/6/2016</t>
+  </si>
+  <si>
+    <t>24/6/2017</t>
+  </si>
+  <si>
+    <t>25/6/2016</t>
+  </si>
+  <si>
+    <t>25/6/2017</t>
+  </si>
+  <si>
+    <t>Trần Long Sơn</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Tổng thời gian</t>
+  </si>
+  <si>
+    <t>Tổng thời gian:</t>
   </si>
 </sst>
 </file>
@@ -531,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,109 +628,109 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>1359037</v>
+        <v>1159032</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>1359038</v>
+        <v>1159032</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>1159032</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1359037</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>1359037</v>
+        <v>1159032</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>1359038</v>
+        <v>1359037</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>1359038</v>
+        <v>1359037</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>1359037</v>
@@ -679,12 +742,12 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>1359037</v>
@@ -696,18 +759,18 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>1359038</v>
+        <v>1359037</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -786,13 +849,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>1159032</v>
+        <v>1359037</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -803,58 +866,58 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>1159032</v>
+        <v>1359037</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17">
-        <v>1159032</v>
+        <v>1359037</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B18">
-        <v>1159032</v>
+        <v>1359037</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1359037</v>
@@ -866,12 +929,12 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>1359037</v>
@@ -880,15 +943,15 @@
         <v>7</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>1359037</v>
@@ -897,15 +960,15 @@
         <v>7</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>1359037</v>
@@ -914,30 +977,204 @@
         <v>7</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>1359037</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>1359037</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>1359037</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>1359037</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>1359037</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>1359037</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>1359038</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>1359037</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>51</v>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>1359038</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>1359038</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>1359038</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44">
+        <v>1359037</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44">
+        <f xml:space="preserve"> SUM(D6:D28)</f>
+        <v>58.5</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E32">
+    <sortCondition ref="B2:B32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -945,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +1223,7 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>1359037</v>
+        <v>1159032</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -994,16 +1231,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D3">
-        <v>1359038</v>
+        <v>1159032</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1011,13 +1248,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>1159032</v>
@@ -1028,36 +1265,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <v>1359037</v>
+        <v>1159032</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42557</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D6">
-        <v>1359038</v>
+        <v>1159032</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1065,16 +1302,16 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>1359037</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1082,10 +1319,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>1359037</v>
@@ -1096,36 +1333,36 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>1359037</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>1359038</v>
+        <v>1359037</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1139,7 +1376,7 @@
         <v>18</v>
       </c>
       <c r="D11">
-        <v>1159032</v>
+        <v>1359037</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1156,7 +1393,7 @@
         <v>25</v>
       </c>
       <c r="D12">
-        <v>1359038</v>
+        <v>1359037</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1167,30 +1404,30 @@
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>1359037</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <v>42406</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D14">
-        <v>1159032</v>
+        <v>1359037</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1198,33 +1435,33 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="B15" s="2">
+        <v>42406</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>1359037</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
+      </c>
+      <c r="B16" s="3">
+        <v>42496</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>1359038</v>
+        <v>1359037</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1232,30 +1469,30 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="B17" s="2">
+        <v>42588</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>1159032</v>
+        <v>1359037</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2">
-        <v>42406</v>
+        <v>42619</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>1359037</v>
@@ -1266,81 +1503,81 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2">
-        <v>42406</v>
+        <v>42649</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D19">
         <v>1359037</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="3">
-        <v>42496</v>
+        <v>47</v>
+      </c>
+      <c r="B20" s="2">
+        <v>42710</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D20">
         <v>1359037</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2">
-        <v>42557</v>
+        <v>47</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D21">
-        <v>1159032</v>
+        <v>1359037</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="2">
-        <v>42588</v>
+        <v>47</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D22">
         <v>1359037</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="2">
-        <v>42619</v>
+      <c r="B23" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D23">
         <v>1359037</v>
@@ -1353,54 +1590,219 @@
       <c r="A24" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="2">
-        <v>42649</v>
+      <c r="B24" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D24">
         <v>1359037</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="2">
-        <v>42710</v>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D25">
         <v>1359037</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26">
+        <v>1359037</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D26">
-        <v>1359037</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
+      <c r="D27">
+        <v>1359037</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28">
+        <v>1359037</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29">
+        <v>1359037</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30">
+        <v>1359037</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>1359038</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>1359038</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33">
+        <v>1359038</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34">
+        <v>1359038</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35">
+        <v>1359038</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1359037</v>
+      </c>
+      <c r="B45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45">
+        <f>SUM(E7:E30)</f>
+        <v>58.5</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E35">
+    <sortCondition ref="D2:D35"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">

</xml_diff>